<commit_message>
витя 16 01 2025
</commit_message>
<xml_diff>
--- a/Vitia_Ostrovsky/R_Calc_Crang_2024/Data/Crang_2024.xlsx
+++ b/Vitia_Ostrovsky/R_Calc_Crang_2024/Data/Crang_2024.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22190" windowHeight="9180" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22190" windowHeight="9180" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Outline_s" sheetId="13" r:id="rId1"/>
@@ -25,10 +25,9 @@
     <sheet name="Coordinats" sheetId="2" r:id="rId11"/>
     <sheet name="Nor" sheetId="6" r:id="rId12"/>
     <sheet name="Full" sheetId="1" r:id="rId13"/>
-    <sheet name="Лист2" sheetId="19" r:id="rId14"/>
-    <sheet name="нето что надо " sheetId="17" r:id="rId15"/>
-    <sheet name="Лист1" sheetId="18" r:id="rId16"/>
-    <sheet name="Nord" sheetId="9" r:id="rId17"/>
+    <sheet name="Лист3" sheetId="20" r:id="rId14"/>
+    <sheet name="Лист1" sheetId="18" r:id="rId15"/>
+    <sheet name="Nord" sheetId="9" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Full!$A$1:$AE$207</definedName>
@@ -54,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="125">
   <si>
     <t>Area</t>
   </si>
@@ -429,7 +428,7 @@
     <t>Кластер 4</t>
   </si>
   <si>
-    <t>Пищевые объекты</t>
+    <t>variable</t>
   </si>
 </sst>
 </file>
@@ -933,11 +932,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="164449640"/>
-        <c:axId val="35784000"/>
+        <c:axId val="162227032"/>
+        <c:axId val="162227424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="164449640"/>
+        <c:axId val="162227032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -994,12 +993,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35784000"/>
+        <c:crossAx val="162227424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="35784000"/>
+        <c:axId val="162227424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1056,7 +1055,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164449640"/>
+        <c:crossAx val="162227032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1436,11 +1435,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="165188328"/>
-        <c:axId val="165192568"/>
+        <c:axId val="162228208"/>
+        <c:axId val="162227816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="165188328"/>
+        <c:axId val="162228208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1497,12 +1496,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165192568"/>
+        <c:crossAx val="162227816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165192568"/>
+        <c:axId val="162227816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1558,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165188328"/>
+        <c:crossAx val="162228208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5563,8 +5562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE207"/>
   <sheetViews>
-    <sheetView topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="D200" sqref="D200:D207"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D157" sqref="D157:D174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20560,7 +20559,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D157">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E157" t="s">
         <v>40</v>
@@ -20656,7 +20655,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D158">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E158" t="s">
         <v>40</v>
@@ -20752,7 +20751,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D159">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E159" t="s">
         <v>40</v>
@@ -20848,7 +20847,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D160">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E160" t="s">
         <v>40</v>
@@ -20944,7 +20943,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D161">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E161" t="s">
         <v>40</v>
@@ -21040,7 +21039,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D162">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E162" t="s">
         <v>40</v>
@@ -21136,7 +21135,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D163">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E163" t="s">
         <v>40</v>
@@ -21232,7 +21231,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D164">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E164" t="s">
         <v>40</v>
@@ -21328,7 +21327,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D165">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E165" t="s">
         <v>40</v>
@@ -21424,7 +21423,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D166">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E166" t="s">
         <v>40</v>
@@ -21520,7 +21519,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D167">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E167" t="s">
         <v>40</v>
@@ -21616,7 +21615,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D168">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E168" t="s">
         <v>40</v>
@@ -21712,7 +21711,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D169">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E169" t="s">
         <v>40</v>
@@ -21808,7 +21807,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D170">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E170" t="s">
         <v>40</v>
@@ -21904,7 +21903,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D171">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E171" t="s">
         <v>40</v>
@@ -22000,7 +21999,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D172">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E172" t="s">
         <v>40</v>
@@ -22096,7 +22095,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D173">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E173" t="s">
         <v>40</v>
@@ -22192,7 +22191,7 @@
         <v>34.351999999999997</v>
       </c>
       <c r="D174">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E174" t="s">
         <v>40</v>
@@ -24016,7 +24015,7 @@
         <v>34.259</v>
       </c>
       <c r="D193">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E193" t="s">
         <v>43</v>
@@ -24112,7 +24111,7 @@
         <v>34.259</v>
       </c>
       <c r="D194">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E194" t="s">
         <v>43</v>
@@ -24208,7 +24207,7 @@
         <v>34.259</v>
       </c>
       <c r="D195">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E195" t="s">
         <v>43</v>
@@ -24304,7 +24303,7 @@
         <v>34.259</v>
       </c>
       <c r="D196">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E196" t="s">
         <v>43</v>
@@ -24400,7 +24399,7 @@
         <v>34.259</v>
       </c>
       <c r="D197">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E197" t="s">
         <v>43</v>
@@ -24496,7 +24495,7 @@
         <v>34.259</v>
       </c>
       <c r="D198">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E198" t="s">
         <v>43</v>
@@ -24592,7 +24591,7 @@
         <v>34.259</v>
       </c>
       <c r="D199">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E199" t="s">
         <v>43</v>
@@ -25454,20 +25453,23 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:F23"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -25481,11 +25483,8 @@
       <c r="E1">
         <v>4</v>
       </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -25499,35 +25498,29 @@
         <v>0.4</v>
       </c>
       <c r="E2">
-        <v>0.7</v>
-      </c>
-      <c r="F2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>0.1</v>
       </c>
       <c r="C3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -25536,138 +25529,165 @@
         <v>0.2</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D5">
         <v>0.2</v>
       </c>
       <c r="E5">
-        <v>0.2</v>
-      </c>
-      <c r="F5">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>0.1</v>
       </c>
       <c r="D6">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="E6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+      <c r="E7">
+        <v>0.1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.1</v>
+      </c>
+      <c r="C8">
         <v>0.2</v>
       </c>
-      <c r="F6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0.2</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
         <v>0.1</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" t="s">
         <v>14</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0.1</v>
-      </c>
-      <c r="D8">
-        <v>0.1</v>
-      </c>
-      <c r="E8">
-        <v>0.1</v>
-      </c>
-      <c r="F8">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0.1</v>
-      </c>
-      <c r="D9">
-        <v>0.2</v>
-      </c>
-      <c r="E9">
-        <v>0.1</v>
-      </c>
-      <c r="F9">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="O10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>12</v>
-      </c>
-      <c r="B10">
-        <v>0.1</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>26</v>
       </c>
       <c r="B11">
         <v>0.1</v>
@@ -25681,154 +25701,145 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>0.1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0.1</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
       <c r="B19">
         <v>0</v>
       </c>
@@ -25836,16 +25847,13 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -25861,11 +25869,8 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -25881,11 +25886,8 @@
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -25901,11 +25903,8 @@
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -25921,1262 +25920,22 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F23">
-    <sortCondition descending="1" ref="C2:C23"/>
+  <sortState ref="A3:E23">
+    <sortCondition descending="1" ref="E3:E23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.90625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-      <c r="N1">
-        <v>13</v>
-      </c>
-      <c r="O1">
-        <v>14</v>
-      </c>
-      <c r="P1">
-        <v>15</v>
-      </c>
-      <c r="Q1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>0.4</v>
-      </c>
-      <c r="C2">
-        <v>0.7</v>
-      </c>
-      <c r="D2">
-        <v>0.7</v>
-      </c>
-      <c r="E2">
-        <v>0.9</v>
-      </c>
-      <c r="F2">
-        <v>0.8</v>
-      </c>
-      <c r="G2">
-        <v>0.6</v>
-      </c>
-      <c r="H2">
-        <v>0.5</v>
-      </c>
-      <c r="I2">
-        <v>0.5</v>
-      </c>
-      <c r="J2">
-        <v>0.3</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0.4</v>
-      </c>
-      <c r="M2">
-        <v>0.2</v>
-      </c>
-      <c r="N2">
-        <v>0.2</v>
-      </c>
-      <c r="O2">
-        <v>0.4</v>
-      </c>
-      <c r="P2">
-        <v>0.6</v>
-      </c>
-      <c r="Q2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>0.5</v>
-      </c>
-      <c r="C3">
-        <v>0.1</v>
-      </c>
-      <c r="D3">
-        <v>0.1</v>
-      </c>
-      <c r="E3">
-        <v>0.1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0.1</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0.1</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>0.1</v>
-      </c>
-      <c r="C4">
-        <v>0.1</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0.1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>0.2</v>
-      </c>
-      <c r="C5">
-        <v>0.1</v>
-      </c>
-      <c r="D5">
-        <v>0.3</v>
-      </c>
-      <c r="E5">
-        <v>0.1</v>
-      </c>
-      <c r="F5">
-        <v>0.1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>0.1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0.1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0.1</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>0.3</v>
-      </c>
-      <c r="C7">
-        <v>0.1</v>
-      </c>
-      <c r="D7">
-        <v>0.1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0.1</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0.2</v>
-      </c>
-      <c r="I7">
-        <v>0.1</v>
-      </c>
-      <c r="J7">
-        <v>0.3</v>
-      </c>
-      <c r="K7">
-        <v>0.2</v>
-      </c>
-      <c r="L7">
-        <v>0.2</v>
-      </c>
-      <c r="M7">
-        <v>0.4</v>
-      </c>
-      <c r="N7">
-        <v>0.2</v>
-      </c>
-      <c r="O7">
-        <v>0.4</v>
-      </c>
-      <c r="P7">
-        <v>0.1</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>0.1</v>
-      </c>
-      <c r="C8">
-        <v>0.1</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0.1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0.1</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0.2</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0.1</v>
-      </c>
-      <c r="M8">
-        <v>0.2</v>
-      </c>
-      <c r="N8">
-        <v>0.3</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0.1</v>
-      </c>
-      <c r="Q8">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>0.2</v>
-      </c>
-      <c r="C9">
-        <v>0.1</v>
-      </c>
-      <c r="D9">
-        <v>0.1</v>
-      </c>
-      <c r="E9">
-        <v>0.1</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0.2</v>
-      </c>
-      <c r="H9">
-        <v>0.1</v>
-      </c>
-      <c r="I9">
-        <v>0.3</v>
-      </c>
-      <c r="J9">
-        <v>0.3</v>
-      </c>
-      <c r="K9">
-        <v>0.5</v>
-      </c>
-      <c r="L9">
-        <v>0.4</v>
-      </c>
-      <c r="M9">
-        <v>0.7</v>
-      </c>
-      <c r="N9">
-        <v>0.5</v>
-      </c>
-      <c r="O9">
-        <v>0.6</v>
-      </c>
-      <c r="P9">
-        <v>0.4</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <v>0.1</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <v>0.1</v>
-      </c>
-      <c r="C11">
-        <v>0.1</v>
-      </c>
-      <c r="D11">
-        <v>0.2</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0.2</v>
-      </c>
-      <c r="I11">
-        <v>0.2</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0.2</v>
-      </c>
-      <c r="L11">
-        <v>0.2</v>
-      </c>
-      <c r="M11">
-        <v>0.2</v>
-      </c>
-      <c r="N11">
-        <v>0.3</v>
-      </c>
-      <c r="O11">
-        <v>0.2</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0.1</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13">
-        <v>0.1</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0.1</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14">
-        <v>0.1</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0.1</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0.1</v>
-      </c>
-      <c r="E18">
-        <v>0.1</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0.1</v>
-      </c>
-      <c r="I18">
-        <v>0.1</v>
-      </c>
-      <c r="J18">
-        <v>0.2</v>
-      </c>
-      <c r="K18">
-        <v>0.2</v>
-      </c>
-      <c r="L18">
-        <v>0.1</v>
-      </c>
-      <c r="M18">
-        <v>0.1</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0.1</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0.1</v>
-      </c>
-      <c r="G20">
-        <v>0.1</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0.1</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0.1</v>
-      </c>
-      <c r="I21">
-        <v>0.1</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>0.1</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0.1</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0.1</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
-  <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection sqref="A1:C23"/>
+      <selection activeCell="A3" sqref="A3:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27208,84 +25967,84 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>0.1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>0.1</v>
-      </c>
-      <c r="C7">
-        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>0.1</v>
       </c>
       <c r="C8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C9">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -27296,18 +26055,18 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -27318,7 +26077,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -27329,7 +26088,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -27340,7 +26099,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -27351,7 +26110,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -27362,7 +26121,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -27373,13 +26132,13 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -27438,11 +26197,14 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C23">
+    <sortCondition descending="1" ref="C2:C23"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B72"/>
   <sheetViews>

</xml_diff>